<commit_message>
Test updates, also made icon protocol agnostic
</commit_message>
<xml_diff>
--- a/test/data/HOLLIS_Links_001787337.xlsx
+++ b/test/data/HOLLIS_Links_001787337.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="150" windowWidth="16500" windowHeight="11415"/>
+    <workbookView xWindow="1220" yWindow="160" windowWidth="16500" windowHeight="11420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Call No:</t>
   </si>
@@ -38,9 +38,6 @@
     <t>CONTENT_LIST</t>
   </si>
   <si>
-    <t>http://hollis.harvard.edu/?itemid=|library/m/aleph|001787337</t>
-  </si>
-  <si>
     <t>http://fts.lib.harvard.edu/fts/search?Q=boston&amp;S=APA</t>
   </si>
   <si>
@@ -114,6 +111,18 @@
   </si>
   <si>
     <t>http://nrs.harvard.edu/urn-3:HLS.LIBR:10873499</t>
+  </si>
+  <si>
+    <t>EXT_ID_TYPE</t>
+  </si>
+  <si>
+    <t>hollis</t>
+  </si>
+  <si>
+    <t>EXT_ID</t>
+  </si>
+  <si>
+    <t>001787337</t>
   </si>
 </sst>
 </file>
@@ -163,11 +172,8 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -175,13 +181,13 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -484,227 +490,234 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2">
+        <v>1915</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>1915</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="2">
+        <v>1916</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>1916</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="2">
+        <v>1917</v>
+      </c>
+      <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>1917</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="2">
+        <v>1927</v>
+      </c>
+      <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>1927</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="2">
+        <v>1928</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>1928</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="2">
+        <v>1929</v>
+      </c>
+      <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>1929</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="2">
+        <v>1930</v>
+      </c>
+      <c r="B15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>1930</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="2">
+        <v>1943</v>
+      </c>
+      <c r="B16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>1943</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="2">
+        <v>1944</v>
+      </c>
+      <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>1944</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="2">
+        <v>1945</v>
+      </c>
+      <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>1945</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="2">
+        <v>1946</v>
+      </c>
+      <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>1946</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="2">
+        <v>1947</v>
+      </c>
+      <c r="B20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>1947</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="2">
+        <v>1948</v>
+      </c>
+      <c r="B21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>1948</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="2">
+        <v>1949</v>
+      </c>
+      <c r="B22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>1949</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="2">
+        <v>1950</v>
+      </c>
+      <c r="B23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>1950</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="2">
+        <v>1951</v>
+      </c>
+      <c r="B24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>1951</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="2">
+        <v>1952</v>
+      </c>
+      <c r="B25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>1952</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="2">
+        <v>1953</v>
+      </c>
+      <c r="B26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>1953</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="2">
+        <v>1954</v>
+      </c>
+      <c r="B27" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>1954</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -722,7 +735,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -739,7 +752,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>